<commit_message>
do data cleaning before applying filters
</commit_message>
<xml_diff>
--- a/files/filterByPatternDatas.xlsx
+++ b/files/filterByPatternDatas.xlsx
@@ -413,7 +413,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>용역 발주계획목록 번호</v>
+        <v>용역 발주계획목록</v>
       </c>
       <c r="B1" t="str">
         <v>업무</v>
@@ -477,8 +477,8 @@
       <c r="H2" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I2" t="str">
-        <v>483,561,215</v>
+      <c r="I2">
+        <v>483561215</v>
       </c>
       <c r="J2" t="str">
         <v>김정철</v>
@@ -512,8 +512,8 @@
       <c r="H3" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I3" t="str">
-        <v>40,000,000</v>
+      <c r="I3">
+        <v>40000000</v>
       </c>
       <c r="J3" t="str">
         <v>정영석</v>
@@ -547,8 +547,8 @@
       <c r="H4" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I4" t="str">
-        <v>530,000,000</v>
+      <c r="I4">
+        <v>530000000</v>
       </c>
       <c r="J4" t="str">
         <v>이경주</v>
@@ -582,8 +582,8 @@
       <c r="H5" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I5" t="str">
-        <v>186,260,000</v>
+      <c r="I5">
+        <v>186260000</v>
       </c>
       <c r="J5" t="str">
         <v>윤연상</v>
@@ -617,8 +617,8 @@
       <c r="H6" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I6" t="str">
-        <v>530,000,000</v>
+      <c r="I6">
+        <v>530000000</v>
       </c>
       <c r="J6" t="str">
         <v>이경주</v>
@@ -652,8 +652,8 @@
       <c r="H7" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I7" t="str">
-        <v>51,139,000</v>
+      <c r="I7">
+        <v>51139000</v>
       </c>
       <c r="J7" t="str">
         <v>엄태웅</v>
@@ -690,8 +690,8 @@
       <c r="H8" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I8" t="str">
-        <v>3,224,342,000</v>
+      <c r="I8">
+        <v>3224342000</v>
       </c>
       <c r="K8" t="str">
         <v>0315106730</v>
@@ -725,8 +725,8 @@
       <c r="H9" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I9" t="str">
-        <v>806,940,000</v>
+      <c r="I9">
+        <v>806940000</v>
       </c>
       <c r="J9" t="str">
         <v>김길규</v>
@@ -766,8 +766,8 @@
       <c r="H10" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I10" t="str">
-        <v>574,300,000</v>
+      <c r="I10">
+        <v>574300000</v>
       </c>
       <c r="J10" t="str">
         <v>김상수</v>
@@ -807,8 +807,8 @@
       <c r="H11" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I11" t="str">
-        <v>40,000,000</v>
+      <c r="I11">
+        <v>40000000</v>
       </c>
       <c r="J11" t="str">
         <v>김태현</v>
@@ -848,8 +848,8 @@
       <c r="H12" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I12" t="str">
-        <v>1,327,941,000</v>
+      <c r="I12">
+        <v>1327941000</v>
       </c>
       <c r="J12" t="str">
         <v>이승연</v>
@@ -889,8 +889,8 @@
       <c r="H13" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I13" t="str">
-        <v>248,656,800</v>
+      <c r="I13">
+        <v>248656800</v>
       </c>
       <c r="J13" t="str">
         <v>박윤진</v>
@@ -930,7 +930,7 @@
       <c r="H14" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I14" t="str">
+      <c r="I14">
         <v>0</v>
       </c>
     </row>
@@ -959,8 +959,8 @@
       <c r="H15" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I15" t="str">
-        <v>321,245,650</v>
+      <c r="I15">
+        <v>321245650</v>
       </c>
       <c r="J15" t="str">
         <v>전민석</v>
@@ -1000,8 +1000,8 @@
       <c r="H16" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I16" t="str">
-        <v>266,000,000</v>
+      <c r="I16">
+        <v>266000000</v>
       </c>
       <c r="J16" t="str">
         <v>손동욱</v>
@@ -1041,8 +1041,8 @@
       <c r="H17" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I17" t="str">
-        <v>428,822,000</v>
+      <c r="I17">
+        <v>428822000</v>
       </c>
       <c r="J17" t="str">
         <v>박천규</v>
@@ -1082,8 +1082,8 @@
       <c r="H18" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I18" t="str">
-        <v>1,199,996,000</v>
+      <c r="I18">
+        <v>1199996000</v>
       </c>
       <c r="J18" t="str">
         <v>이병완</v>
@@ -1123,8 +1123,8 @@
       <c r="H19" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I19" t="str">
-        <v>340,000,000</v>
+      <c r="I19">
+        <v>340000000</v>
       </c>
       <c r="J19" t="str">
         <v>신희은</v>
@@ -1159,13 +1159,13 @@
         <v>일반경쟁</v>
       </c>
       <c r="G20" t="str">
-        <v>경부고속도로 직선화 공사(우회도로  3, 4) 건설사업관리용역</v>
+        <v>경부고속도로 직선화 공사(우회도로 3, 4) 건설사업관리용역</v>
       </c>
       <c r="H20" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I20" t="str">
-        <v>455,000,000</v>
+      <c r="I20">
+        <v>455000000</v>
       </c>
       <c r="J20" t="str">
         <v>정재훈</v>
@@ -1202,8 +1202,8 @@
       <c r="H21" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I21" t="str">
-        <v>1,312,000,000</v>
+      <c r="I21">
+        <v>1312000000</v>
       </c>
       <c r="J21" t="str">
         <v>이병주</v>
@@ -1243,8 +1243,8 @@
       <c r="H22" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I22" t="str">
-        <v>86,300,000</v>
+      <c r="I22">
+        <v>86300000</v>
       </c>
       <c r="J22" t="str">
         <v>김상우</v>
@@ -1284,8 +1284,8 @@
       <c r="H23" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I23" t="str">
-        <v>99,200,000</v>
+      <c r="I23">
+        <v>99200000</v>
       </c>
       <c r="J23" t="str">
         <v>원창빈</v>
@@ -1325,8 +1325,8 @@
       <c r="H24" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I24" t="str">
-        <v>140,000,000</v>
+      <c r="I24">
+        <v>140000000</v>
       </c>
       <c r="J24" t="str">
         <v>김수진</v>
@@ -1366,8 +1366,8 @@
       <c r="H25" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I25" t="str">
-        <v>56,650,000</v>
+      <c r="I25">
+        <v>56650000</v>
       </c>
       <c r="J25" t="str">
         <v>박소희</v>
@@ -1407,8 +1407,8 @@
       <c r="H26" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I26" t="str">
-        <v>168,840,000</v>
+      <c r="I26">
+        <v>168840000</v>
       </c>
       <c r="J26" t="str">
         <v>서동주</v>
@@ -1448,8 +1448,8 @@
       <c r="H27" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I27" t="str">
-        <v>153,970,000</v>
+      <c r="I27">
+        <v>153970000</v>
       </c>
       <c r="J27" t="str">
         <v>안영주</v>
@@ -1489,8 +1489,8 @@
       <c r="H28" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I28" t="str">
-        <v>599,849,760</v>
+      <c r="I28">
+        <v>599849760</v>
       </c>
       <c r="J28" t="str">
         <v>심용준</v>
@@ -1530,8 +1530,8 @@
       <c r="H29" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I29" t="str">
-        <v>1,115,400,000</v>
+      <c r="I29">
+        <v>1115400000</v>
       </c>
       <c r="J29" t="str">
         <v>전민서</v>
@@ -1571,7 +1571,7 @@
       <c r="H30" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I30" t="str">
+      <c r="I30">
         <v>0</v>
       </c>
     </row>
@@ -1600,8 +1600,8 @@
       <c r="H31" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I31" t="str">
-        <v>46,000,000</v>
+      <c r="I31">
+        <v>46000000</v>
       </c>
       <c r="J31" t="str">
         <v>김수진</v>
@@ -1641,8 +1641,8 @@
       <c r="H32" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I32" t="str">
-        <v>440,000,000</v>
+      <c r="I32">
+        <v>440000000</v>
       </c>
       <c r="J32" t="str">
         <v>임현숙</v>
@@ -1679,8 +1679,8 @@
       <c r="H33" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I33" t="str">
-        <v>130,000,000</v>
+      <c r="I33">
+        <v>130000000</v>
       </c>
       <c r="J33" t="str">
         <v>김수진</v>
@@ -1720,8 +1720,8 @@
       <c r="H34" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I34" t="str">
-        <v>190,000,000</v>
+      <c r="I34">
+        <v>190000000</v>
       </c>
       <c r="J34" t="str">
         <v>금지윤</v>
@@ -1761,8 +1761,8 @@
       <c r="H35" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I35" t="str">
-        <v>75,150,000</v>
+      <c r="I35">
+        <v>75150000</v>
       </c>
       <c r="J35" t="str">
         <v>유수안</v>
@@ -1802,8 +1802,8 @@
       <c r="H36" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I36" t="str">
-        <v>100,000,000</v>
+      <c r="I36">
+        <v>100000000</v>
       </c>
       <c r="J36" t="str">
         <v>김수진</v>
@@ -1843,8 +1843,8 @@
       <c r="H37" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I37" t="str">
-        <v>59,000,000</v>
+      <c r="I37">
+        <v>59000000</v>
       </c>
       <c r="J37" t="str">
         <v>이현용</v>
@@ -1884,8 +1884,8 @@
       <c r="H38" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I38" t="str">
-        <v>300,000,000</v>
+      <c r="I38">
+        <v>300000000</v>
       </c>
       <c r="J38" t="str">
         <v>사현지</v>
@@ -1925,8 +1925,8 @@
       <c r="H39" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I39" t="str">
-        <v>111,170,000</v>
+      <c r="I39">
+        <v>111170000</v>
       </c>
       <c r="J39" t="str">
         <v>강진우</v>
@@ -1966,8 +1966,8 @@
       <c r="H40" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I40" t="str">
-        <v>130,000,000</v>
+      <c r="I40">
+        <v>130000000</v>
       </c>
       <c r="J40" t="str">
         <v>김수진</v>
@@ -2007,8 +2007,8 @@
       <c r="H41" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I41" t="str">
-        <v>1,436,644,000</v>
+      <c r="I41">
+        <v>1436644000</v>
       </c>
       <c r="J41" t="str">
         <v>이상락</v>
@@ -2048,8 +2048,8 @@
       <c r="H42" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I42" t="str">
-        <v>128,000,000</v>
+      <c r="I42">
+        <v>128000000</v>
       </c>
       <c r="J42" t="str">
         <v>과장 정영학</v>
@@ -2089,8 +2089,8 @@
       <c r="H43" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I43" t="str">
-        <v>8,600,500,000</v>
+      <c r="I43">
+        <v>8600500000</v>
       </c>
       <c r="J43" t="str">
         <v>유상호</v>
@@ -2130,8 +2130,8 @@
       <c r="H44" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I44" t="str">
-        <v>130,000,000</v>
+      <c r="I44">
+        <v>130000000</v>
       </c>
       <c r="J44" t="str">
         <v>김수진</v>
@@ -2171,8 +2171,8 @@
       <c r="H45" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I45" t="str">
-        <v>100,000,000</v>
+      <c r="I45">
+        <v>100000000</v>
       </c>
       <c r="J45" t="str">
         <v>김희나</v>
@@ -2212,8 +2212,8 @@
       <c r="H46" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I46" t="str">
-        <v>100,000,000</v>
+      <c r="I46">
+        <v>100000000</v>
       </c>
       <c r="J46" t="str">
         <v>김수진</v>
@@ -2253,8 +2253,8 @@
       <c r="H47" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I47" t="str">
-        <v>1,184,481,000</v>
+      <c r="I47">
+        <v>1184481000</v>
       </c>
       <c r="J47" t="str">
         <v>과장 김택효</v>
@@ -2294,8 +2294,8 @@
       <c r="H48" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I48" t="str">
-        <v>100,000,000</v>
+      <c r="I48">
+        <v>100000000</v>
       </c>
       <c r="J48" t="str">
         <v>김수진</v>
@@ -2335,8 +2335,8 @@
       <c r="H49" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I49" t="str">
-        <v>638,220,000</v>
+      <c r="I49">
+        <v>638220000</v>
       </c>
       <c r="J49" t="str">
         <v>이근행</v>
@@ -2376,8 +2376,8 @@
       <c r="H50" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I50" t="str">
-        <v>2,232,000,000</v>
+      <c r="I50">
+        <v>2232000000</v>
       </c>
       <c r="J50" t="str">
         <v>오아름</v>
@@ -2417,8 +2417,8 @@
       <c r="H51" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I51" t="str">
-        <v>633,600,000</v>
+      <c r="I51">
+        <v>633600000</v>
       </c>
       <c r="J51" t="str">
         <v>오석환</v>
@@ -2458,8 +2458,8 @@
       <c r="H52" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I52" t="str">
-        <v>95,000,000</v>
+      <c r="I52">
+        <v>95000000</v>
       </c>
       <c r="J52" t="str">
         <v>김영아</v>
@@ -2499,8 +2499,8 @@
       <c r="H53" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I53" t="str">
-        <v>100,000,000</v>
+      <c r="I53">
+        <v>100000000</v>
       </c>
       <c r="J53" t="str">
         <v>김영아</v>
@@ -2540,8 +2540,8 @@
       <c r="H54" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I54" t="str">
-        <v>200,000,000</v>
+      <c r="I54">
+        <v>200000000</v>
       </c>
       <c r="J54" t="str">
         <v>채수민</v>
@@ -2581,8 +2581,8 @@
       <c r="H55" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I55" t="str">
-        <v>70,500,000</v>
+      <c r="I55">
+        <v>70500000</v>
       </c>
       <c r="J55" t="str">
         <v>임동혁</v>
@@ -2622,8 +2622,8 @@
       <c r="H56" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I56" t="str">
-        <v>1,083,400,000</v>
+      <c r="I56">
+        <v>1083400000</v>
       </c>
       <c r="J56" t="str">
         <v>김동영</v>
@@ -2663,8 +2663,8 @@
       <c r="H57" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I57" t="str">
-        <v>1,311,861,000</v>
+      <c r="I57">
+        <v>1311861000</v>
       </c>
       <c r="J57" t="str">
         <v>차장 이인석</v>
@@ -2704,8 +2704,8 @@
       <c r="H58" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I58" t="str">
-        <v>30,000,000</v>
+      <c r="I58">
+        <v>30000000</v>
       </c>
       <c r="J58" t="str">
         <v>손병동</v>
@@ -2745,8 +2745,8 @@
       <c r="H59" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I59" t="str">
-        <v>70,000,000</v>
+      <c r="I59">
+        <v>70000000</v>
       </c>
       <c r="J59" t="str">
         <v>박현규</v>
@@ -2786,8 +2786,8 @@
       <c r="H60" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I60" t="str">
-        <v>459,976,000</v>
+      <c r="I60">
+        <v>459976000</v>
       </c>
       <c r="J60" t="str">
         <v>한빛나</v>
@@ -2827,8 +2827,8 @@
       <c r="H61" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I61" t="str">
-        <v>765,081,193</v>
+      <c r="I61">
+        <v>765081193</v>
       </c>
       <c r="J61" t="str">
         <v>홍혜선</v>
@@ -2868,8 +2868,8 @@
       <c r="H62" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I62" t="str">
-        <v>73,200,000</v>
+      <c r="I62">
+        <v>73200000</v>
       </c>
       <c r="J62" t="str">
         <v>홍은비</v>
@@ -2909,8 +2909,8 @@
       <c r="H63" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I63" t="str">
-        <v>25,000,000</v>
+      <c r="I63">
+        <v>25000000</v>
       </c>
       <c r="J63" t="str">
         <v>김동규</v>
@@ -2950,8 +2950,8 @@
       <c r="H64" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I64" t="str">
-        <v>390,352,000</v>
+      <c r="I64">
+        <v>390352000</v>
       </c>
       <c r="J64" t="str">
         <v>이은진</v>
@@ -2991,8 +2991,8 @@
       <c r="H65" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I65" t="str">
-        <v>1,529,000,000</v>
+      <c r="I65">
+        <v>1529000000</v>
       </c>
       <c r="J65" t="str">
         <v>광성조</v>
@@ -3032,8 +3032,8 @@
       <c r="H66" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I66" t="str">
-        <v>365,828,800</v>
+      <c r="I66">
+        <v>365828800</v>
       </c>
     </row>
     <row r="67">
@@ -3061,8 +3061,8 @@
       <c r="H67" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I67" t="str">
-        <v>100,000,000</v>
+      <c r="I67">
+        <v>100000000</v>
       </c>
       <c r="J67" t="str">
         <v>엄정호</v>
@@ -3102,8 +3102,8 @@
       <c r="H68" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I68" t="str">
-        <v>182,600,000</v>
+      <c r="I68">
+        <v>182600000</v>
       </c>
       <c r="J68" t="str">
         <v>정수형</v>
@@ -3143,8 +3143,8 @@
       <c r="H69" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I69" t="str">
-        <v>39,424,000</v>
+      <c r="I69">
+        <v>39424000</v>
       </c>
       <c r="J69" t="str">
         <v>류미지</v>
@@ -3184,8 +3184,8 @@
       <c r="H70" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I70" t="str">
-        <v>87,868,000</v>
+      <c r="I70">
+        <v>87868000</v>
       </c>
       <c r="J70" t="str">
         <v>전봉준</v>
@@ -3225,8 +3225,8 @@
       <c r="H71" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I71" t="str">
-        <v>25,300,000</v>
+      <c r="I71">
+        <v>25300000</v>
       </c>
       <c r="J71" t="str">
         <v>최대인</v>
@@ -3266,8 +3266,8 @@
       <c r="H72" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I72" t="str">
-        <v>420,000,000</v>
+      <c r="I72">
+        <v>420000000</v>
       </c>
       <c r="J72" t="str">
         <v>김형순</v>
@@ -3307,8 +3307,8 @@
       <c r="H73" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I73" t="str">
-        <v>36,000,000</v>
+      <c r="I73">
+        <v>36000000</v>
       </c>
       <c r="J73" t="str">
         <v>신성호</v>
@@ -3348,8 +3348,8 @@
       <c r="H74" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I74" t="str">
-        <v>48,972,000</v>
+      <c r="I74">
+        <v>48972000</v>
       </c>
       <c r="J74" t="str">
         <v>권민영</v>
@@ -3389,8 +3389,8 @@
       <c r="H75" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I75" t="str">
-        <v>65,650,000</v>
+      <c r="I75">
+        <v>65650000</v>
       </c>
       <c r="J75" t="str">
         <v>손현정</v>
@@ -3430,8 +3430,8 @@
       <c r="H76" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I76" t="str">
-        <v>470,392,000</v>
+      <c r="I76">
+        <v>470392000</v>
       </c>
       <c r="J76" t="str">
         <v>권은혜</v>
@@ -3471,8 +3471,8 @@
       <c r="H77" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I77" t="str">
-        <v>385,000,000</v>
+      <c r="I77">
+        <v>385000000</v>
       </c>
       <c r="J77" t="str">
         <v>하동수</v>
@@ -3512,8 +3512,8 @@
       <c r="H78" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I78" t="str">
-        <v>2,502,000,000</v>
+      <c r="I78">
+        <v>2502000000</v>
       </c>
       <c r="J78" t="str">
         <v>정진이</v>
@@ -3553,8 +3553,8 @@
       <c r="H79" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I79" t="str">
-        <v>55,000,000</v>
+      <c r="I79">
+        <v>55000000</v>
       </c>
       <c r="J79" t="str">
         <v>김우진</v>
@@ -3594,8 +3594,8 @@
       <c r="H80" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I80" t="str">
-        <v>1,595,920,000</v>
+      <c r="I80">
+        <v>1595920000</v>
       </c>
       <c r="J80" t="str">
         <v>김희창</v>
@@ -3635,8 +3635,8 @@
       <c r="H81" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I81" t="str">
-        <v>200,000,000</v>
+      <c r="I81">
+        <v>200000000</v>
       </c>
       <c r="J81" t="str">
         <v>양병욱</v>
@@ -3676,8 +3676,8 @@
       <c r="H82" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I82" t="str">
-        <v>192,896,000</v>
+      <c r="I82">
+        <v>192896000</v>
       </c>
       <c r="J82" t="str">
         <v>박찬미</v>
@@ -3717,8 +3717,8 @@
       <c r="H83" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I83" t="str">
-        <v>120,000,000</v>
+      <c r="I83">
+        <v>120000000</v>
       </c>
       <c r="J83" t="str">
         <v>배승준</v>
@@ -3758,8 +3758,8 @@
       <c r="H84" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I84" t="str">
-        <v>596,103,920</v>
+      <c r="I84">
+        <v>596103920</v>
       </c>
       <c r="J84" t="str">
         <v>손주환</v>
@@ -3799,8 +3799,8 @@
       <c r="H85" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I85" t="str">
-        <v>4,537,720,000</v>
+      <c r="I85">
+        <v>4537720000</v>
       </c>
       <c r="J85" t="str">
         <v>이해경</v>
@@ -3840,8 +3840,8 @@
       <c r="H86" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I86" t="str">
-        <v>476,570,000</v>
+      <c r="I86">
+        <v>476570000</v>
       </c>
       <c r="J86" t="str">
         <v>양명완</v>
@@ -3881,8 +3881,8 @@
       <c r="H87" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I87" t="str">
-        <v>704,760,000</v>
+      <c r="I87">
+        <v>704760000</v>
       </c>
       <c r="J87" t="str">
         <v>서유경</v>
@@ -3922,8 +3922,8 @@
       <c r="H88" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I88" t="str">
-        <v>168,230,000</v>
+      <c r="I88">
+        <v>168230000</v>
       </c>
       <c r="J88" t="str">
         <v>이희문</v>
@@ -3963,8 +3963,8 @@
       <c r="H89" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I89" t="str">
-        <v>30,000,000</v>
+      <c r="I89">
+        <v>30000000</v>
       </c>
       <c r="J89" t="str">
         <v>박민호</v>
@@ -4004,8 +4004,8 @@
       <c r="H90" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I90" t="str">
-        <v>100,000,000</v>
+      <c r="I90">
+        <v>100000000</v>
       </c>
       <c r="J90" t="str">
         <v>김규빈</v>
@@ -4045,8 +4045,8 @@
       <c r="H91" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I91" t="str">
-        <v>32,000,000</v>
+      <c r="I91">
+        <v>32000000</v>
       </c>
       <c r="J91" t="str">
         <v>송민규</v>
@@ -4086,8 +4086,8 @@
       <c r="H92" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I92" t="str">
-        <v>45,000,000</v>
+      <c r="I92">
+        <v>45000000</v>
       </c>
       <c r="J92" t="str">
         <v>양해솔</v>
@@ -4127,8 +4127,8 @@
       <c r="H93" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I93" t="str">
-        <v>2,840,000,000</v>
+      <c r="I93">
+        <v>2840000000</v>
       </c>
       <c r="J93" t="str">
         <v>이문구</v>
@@ -4168,8 +4168,8 @@
       <c r="H94" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I94" t="str">
-        <v>160,000,000</v>
+      <c r="I94">
+        <v>160000000</v>
       </c>
       <c r="J94" t="str">
         <v>손슬기</v>
@@ -4209,8 +4209,8 @@
       <c r="H95" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I95" t="str">
-        <v>100,000,000</v>
+      <c r="I95">
+        <v>100000000</v>
       </c>
       <c r="J95" t="str">
         <v>손슬기</v>
@@ -4250,8 +4250,8 @@
       <c r="H96" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I96" t="str">
-        <v>100,000,000</v>
+      <c r="I96">
+        <v>100000000</v>
       </c>
       <c r="J96" t="str">
         <v>김소라</v>
@@ -4291,8 +4291,8 @@
       <c r="H97" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I97" t="str">
-        <v>180,000,000</v>
+      <c r="I97">
+        <v>180000000</v>
       </c>
       <c r="J97" t="str">
         <v>김소라</v>
@@ -4332,8 +4332,8 @@
       <c r="H98" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I98" t="str">
-        <v>40,187,000</v>
+      <c r="I98">
+        <v>40187000</v>
       </c>
       <c r="J98" t="str">
         <v>윤상우</v>
@@ -4367,8 +4367,8 @@
       <c r="H99" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I99" t="str">
-        <v>32,940,000</v>
+      <c r="I99">
+        <v>32940000</v>
       </c>
       <c r="J99" t="str">
         <v>정종근</v>
@@ -4402,8 +4402,8 @@
       <c r="H100" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I100" t="str">
-        <v>324,551,850</v>
+      <c r="I100">
+        <v>324551850</v>
       </c>
       <c r="J100" t="str">
         <v>성민정</v>
@@ -4437,8 +4437,8 @@
       <c r="H101" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I101" t="str">
-        <v>259,917,900</v>
+      <c r="I101">
+        <v>259917900</v>
       </c>
       <c r="K101" t="str">
         <v>03116708572</v>
@@ -4472,8 +4472,8 @@
       <c r="H102" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I102" t="str">
-        <v>900,000,000</v>
+      <c r="I102">
+        <v>900000000</v>
       </c>
       <c r="J102" t="str">
         <v>인지만</v>
@@ -4513,8 +4513,8 @@
       <c r="H103" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I103" t="str">
-        <v>41,611,000</v>
+      <c r="I103">
+        <v>41611000</v>
       </c>
       <c r="J103" t="str">
         <v>이유진</v>
@@ -4554,8 +4554,8 @@
       <c r="H104" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I104" t="str">
-        <v>38,148,000</v>
+      <c r="I104">
+        <v>38148000</v>
       </c>
       <c r="J104" t="str">
         <v>이유진</v>
@@ -4595,8 +4595,8 @@
       <c r="H105" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I105" t="str">
-        <v>1,263,000,000</v>
+      <c r="I105">
+        <v>1263000000</v>
       </c>
       <c r="J105" t="str">
         <v>신광</v>
@@ -4636,8 +4636,8 @@
       <c r="H106" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I106" t="str">
-        <v>50,000,000</v>
+      <c r="I106">
+        <v>50000000</v>
       </c>
       <c r="J106" t="str">
         <v>배진영</v>
@@ -4677,8 +4677,8 @@
       <c r="H107" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I107" t="str">
-        <v>100,000,000</v>
+      <c r="I107">
+        <v>100000000</v>
       </c>
       <c r="J107" t="str">
         <v>김기표</v>
@@ -4718,8 +4718,8 @@
       <c r="H108" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I108" t="str">
-        <v>272,000,000</v>
+      <c r="I108">
+        <v>272000000</v>
       </c>
       <c r="J108" t="str">
         <v>유승희</v>
@@ -4759,8 +4759,8 @@
       <c r="H109" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I109" t="str">
-        <v>22,000,000</v>
+      <c r="I109">
+        <v>22000000</v>
       </c>
       <c r="J109" t="str">
         <v>유성호</v>
@@ -4800,8 +4800,8 @@
       <c r="H110" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I110" t="str">
-        <v>839,127,000</v>
+      <c r="I110">
+        <v>839127000</v>
       </c>
       <c r="J110" t="str">
         <v>강경이</v>
@@ -4841,8 +4841,8 @@
       <c r="H111" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I111" t="str">
-        <v>278,190,000</v>
+      <c r="I111">
+        <v>278190000</v>
       </c>
       <c r="J111" t="str">
         <v>안주희</v>
@@ -4882,8 +4882,8 @@
       <c r="H112" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I112" t="str">
-        <v>1,942,551,000</v>
+      <c r="I112">
+        <v>1942551000</v>
       </c>
       <c r="J112" t="str">
         <v>강경이</v>
@@ -4923,8 +4923,8 @@
       <c r="H113" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I113" t="str">
-        <v>1,401,677,000</v>
+      <c r="I113">
+        <v>1401677000</v>
       </c>
       <c r="J113" t="str">
         <v>강경이</v>
@@ -4964,8 +4964,8 @@
       <c r="H114" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I114" t="str">
-        <v>1,803,556,000</v>
+      <c r="I114">
+        <v>1803556000</v>
       </c>
       <c r="J114" t="str">
         <v>강경이</v>
@@ -5005,8 +5005,8 @@
       <c r="H115" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I115" t="str">
-        <v>520,000,000</v>
+      <c r="I115">
+        <v>520000000</v>
       </c>
       <c r="J115" t="str">
         <v>한수아</v>
@@ -5046,8 +5046,8 @@
       <c r="H116" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I116" t="str">
-        <v>65,000,000</v>
+      <c r="I116">
+        <v>65000000</v>
       </c>
       <c r="J116" t="str">
         <v>유영아</v>
@@ -5087,8 +5087,8 @@
       <c r="H117" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I117" t="str">
-        <v>200,000,000</v>
+      <c r="I117">
+        <v>200000000</v>
       </c>
       <c r="J117" t="str">
         <v>전유민</v>
@@ -5128,8 +5128,8 @@
       <c r="H118" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I118" t="str">
-        <v>598,521,000</v>
+      <c r="I118">
+        <v>598521000</v>
       </c>
       <c r="J118" t="str">
         <v>이상철</v>
@@ -5169,8 +5169,8 @@
       <c r="H119" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I119" t="str">
-        <v>2,697,000,000</v>
+      <c r="I119">
+        <v>2697000000</v>
       </c>
       <c r="J119" t="str">
         <v>허치도</v>
@@ -5210,8 +5210,8 @@
       <c r="H120" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I120" t="str">
-        <v>67,800,000</v>
+      <c r="I120">
+        <v>67800000</v>
       </c>
       <c r="J120" t="str">
         <v>민승기</v>
@@ -5234,7 +5234,7 @@
         <v>용역</v>
       </c>
       <c r="C121" t="str">
-        <v xml:space="preserve">(사)대한전기협회                                  </v>
+        <v>(사)대한전기협회</v>
       </c>
       <c r="D121" t="str">
         <v>2024년 05월</v>
@@ -5251,8 +5251,8 @@
       <c r="H121" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I121" t="str">
-        <v>100,236,000</v>
+      <c r="I121">
+        <v>100236000</v>
       </c>
       <c r="J121" t="str">
         <v>김문주</v>
@@ -5292,8 +5292,8 @@
       <c r="H122" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I122" t="str">
-        <v>137,800,000</v>
+      <c r="I122">
+        <v>137800000</v>
       </c>
       <c r="J122" t="str">
         <v>황대관</v>
@@ -5333,8 +5333,8 @@
       <c r="H123" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I123" t="str">
-        <v>395,300,000</v>
+      <c r="I123">
+        <v>395300000</v>
       </c>
       <c r="J123" t="str">
         <v>최수연</v>
@@ -5374,8 +5374,8 @@
       <c r="H124" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I124" t="str">
-        <v>443,000,000</v>
+      <c r="I124">
+        <v>443000000</v>
       </c>
       <c r="J124" t="str">
         <v>김영주</v>
@@ -5415,8 +5415,8 @@
       <c r="H125" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I125" t="str">
-        <v>959,000,000</v>
+      <c r="I125">
+        <v>959000000</v>
       </c>
       <c r="J125" t="str">
         <v>한미연</v>
@@ -5456,8 +5456,8 @@
       <c r="H126" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I126" t="str">
-        <v>440,337,600</v>
+      <c r="I126">
+        <v>440337600</v>
       </c>
       <c r="J126" t="str">
         <v>장초롱</v>
@@ -5497,8 +5497,8 @@
       <c r="H127" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I127" t="str">
-        <v>10,131,000,000</v>
+      <c r="I127">
+        <v>10131000000</v>
       </c>
       <c r="J127" t="str">
         <v>임지혜 사무관</v>
@@ -5538,8 +5538,8 @@
       <c r="H128" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I128" t="str">
-        <v>35,000,000</v>
+      <c r="I128">
+        <v>35000000</v>
       </c>
       <c r="J128" t="str">
         <v>박나영</v>
@@ -5579,8 +5579,8 @@
       <c r="H129" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I129" t="str">
-        <v>60,000,000</v>
+      <c r="I129">
+        <v>60000000</v>
       </c>
       <c r="J129" t="str">
         <v>진현아</v>
@@ -5620,8 +5620,8 @@
       <c r="H130" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I130" t="str">
-        <v>1,993,527,000</v>
+      <c r="I130">
+        <v>1993527000</v>
       </c>
       <c r="J130" t="str">
         <v>이선미</v>
@@ -5661,8 +5661,8 @@
       <c r="H131" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I131" t="str">
-        <v>131,700,000</v>
+      <c r="I131">
+        <v>131700000</v>
       </c>
       <c r="J131" t="str">
         <v>김인태</v>
@@ -5702,8 +5702,8 @@
       <c r="H132" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I132" t="str">
-        <v>24,000,000</v>
+      <c r="I132">
+        <v>24000000</v>
       </c>
       <c r="J132" t="str">
         <v>조민희</v>
@@ -5743,8 +5743,8 @@
       <c r="H133" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I133" t="str">
-        <v>3,341,674,187</v>
+      <c r="I133">
+        <v>3341674187</v>
       </c>
       <c r="J133" t="str">
         <v>홍혜선</v>
@@ -5784,8 +5784,8 @@
       <c r="H134" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I134" t="str">
-        <v>62,000,000</v>
+      <c r="I134">
+        <v>62000000</v>
       </c>
       <c r="J134" t="str">
         <v>김영진</v>
@@ -5825,8 +5825,8 @@
       <c r="H135" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I135" t="str">
-        <v>362,000,000</v>
+      <c r="I135">
+        <v>362000000</v>
       </c>
       <c r="J135" t="str">
         <v>박진주</v>
@@ -5863,8 +5863,8 @@
       <c r="H136" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I136" t="str">
-        <v>215,000,000</v>
+      <c r="I136">
+        <v>215000000</v>
       </c>
       <c r="J136" t="str">
         <v>김완수</v>
@@ -5901,8 +5901,8 @@
       <c r="H137" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I137" t="str">
-        <v>80,000,000</v>
+      <c r="I137">
+        <v>80000000</v>
       </c>
       <c r="J137" t="str">
         <v>김원일</v>
@@ -5942,8 +5942,8 @@
       <c r="H138" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I138" t="str">
-        <v>3,213,520,000</v>
+      <c r="I138">
+        <v>3213520000</v>
       </c>
       <c r="J138" t="str">
         <v>오정은</v>
@@ -5983,8 +5983,8 @@
       <c r="H139" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I139" t="str">
-        <v>160,000,000</v>
+      <c r="I139">
+        <v>160000000</v>
       </c>
       <c r="J139" t="str">
         <v>신현주</v>
@@ -6024,8 +6024,8 @@
       <c r="H140" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I140" t="str">
-        <v>534,551,445</v>
+      <c r="I140">
+        <v>534551445</v>
       </c>
       <c r="J140" t="str">
         <v>신우정</v>
@@ -6065,8 +6065,8 @@
       <c r="H141" t="str">
         <v>기술용역</v>
       </c>
-      <c r="I141" t="str">
-        <v>115,700,000</v>
+      <c r="I141">
+        <v>115700000</v>
       </c>
       <c r="J141" t="str">
         <v>김진철</v>
@@ -6106,8 +6106,8 @@
       <c r="H142" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I142" t="str">
-        <v>60,000,000</v>
+      <c r="I142">
+        <v>60000000</v>
       </c>
       <c r="J142" t="str">
         <v>조연희</v>
@@ -6147,8 +6147,8 @@
       <c r="H143" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I143" t="str">
-        <v>367,400,000</v>
+      <c r="I143">
+        <v>367400000</v>
       </c>
       <c r="J143" t="str">
         <v>정평교</v>
@@ -6188,8 +6188,8 @@
       <c r="H144" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I144" t="str">
-        <v>100,000,000</v>
+      <c r="I144">
+        <v>100000000</v>
       </c>
       <c r="J144" t="str">
         <v>황인성</v>
@@ -6229,8 +6229,8 @@
       <c r="H145" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I145" t="str">
-        <v>99,000,000</v>
+      <c r="I145">
+        <v>99000000</v>
       </c>
       <c r="J145" t="str">
         <v>장준구</v>
@@ -6270,8 +6270,8 @@
       <c r="H146" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I146" t="str">
-        <v>38,500,000</v>
+      <c r="I146">
+        <v>38500000</v>
       </c>
       <c r="J146" t="str">
         <v>이동열</v>
@@ -6311,8 +6311,8 @@
       <c r="H147" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I147" t="str">
-        <v>1,065,000,000</v>
+      <c r="I147">
+        <v>1065000000</v>
       </c>
       <c r="J147" t="str">
         <v>조은미 팀장</v>
@@ -6352,7 +6352,7 @@
       <c r="H148" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I148" t="str">
+      <c r="I148">
         <v>1</v>
       </c>
       <c r="J148" t="str">
@@ -6393,7 +6393,7 @@
       <c r="H149" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I149" t="str">
+      <c r="I149">
         <v>1</v>
       </c>
       <c r="J149" t="str">
@@ -6434,8 +6434,8 @@
       <c r="H150" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I150" t="str">
-        <v>150,000,000</v>
+      <c r="I150">
+        <v>150000000</v>
       </c>
       <c r="J150" t="str">
         <v>김광언</v>
@@ -6475,8 +6475,8 @@
       <c r="H151" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I151" t="str">
-        <v>50,000,000</v>
+      <c r="I151">
+        <v>50000000</v>
       </c>
       <c r="J151" t="str">
         <v>이지웅</v>
@@ -6516,8 +6516,8 @@
       <c r="H152" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I152" t="str">
-        <v>44,840,400</v>
+      <c r="I152">
+        <v>44840400</v>
       </c>
       <c r="J152" t="str">
         <v>장세현</v>
@@ -6557,8 +6557,8 @@
       <c r="H153" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I153" t="str">
-        <v>50,000,000</v>
+      <c r="I153">
+        <v>50000000</v>
       </c>
       <c r="J153" t="str">
         <v>윤형필</v>
@@ -6598,8 +6598,8 @@
       <c r="H154" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I154" t="str">
-        <v>3,310,000,000</v>
+      <c r="I154">
+        <v>3310000000</v>
       </c>
       <c r="J154" t="str">
         <v>임영준</v>
@@ -6639,8 +6639,8 @@
       <c r="H155" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I155" t="str">
-        <v>33,000,000</v>
+      <c r="I155">
+        <v>33000000</v>
       </c>
       <c r="J155" t="str">
         <v>이호진</v>
@@ -6680,8 +6680,8 @@
       <c r="H156" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I156" t="str">
-        <v>300,000,000</v>
+      <c r="I156">
+        <v>300000000</v>
       </c>
       <c r="J156" t="str">
         <v>김영목</v>
@@ -6721,8 +6721,8 @@
       <c r="H157" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I157" t="str">
-        <v>400,000,000</v>
+      <c r="I157">
+        <v>400000000</v>
       </c>
       <c r="J157" t="str">
         <v>이정운</v>
@@ -6762,8 +6762,8 @@
       <c r="H158" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I158" t="str">
-        <v>120,000,000</v>
+      <c r="I158">
+        <v>120000000</v>
       </c>
       <c r="J158" t="str">
         <v>배승준</v>
@@ -6803,8 +6803,8 @@
       <c r="H159" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I159" t="str">
-        <v>40,000,000</v>
+      <c r="I159">
+        <v>40000000</v>
       </c>
       <c r="J159" t="str">
         <v>김민경</v>
@@ -6844,8 +6844,8 @@
       <c r="H160" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I160" t="str">
-        <v>80,000,000</v>
+      <c r="I160">
+        <v>80000000</v>
       </c>
       <c r="J160" t="str">
         <v>선임차장 이승환</v>
@@ -6885,8 +6885,8 @@
       <c r="H161" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I161" t="str">
-        <v>199,767,000</v>
+      <c r="I161">
+        <v>199767000</v>
       </c>
       <c r="J161" t="str">
         <v>신다희</v>
@@ -6926,8 +6926,8 @@
       <c r="H162" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I162" t="str">
-        <v>758,259,000</v>
+      <c r="I162">
+        <v>758259000</v>
       </c>
       <c r="J162" t="str">
         <v>신다희</v>
@@ -6967,8 +6967,8 @@
       <c r="H163" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I163" t="str">
-        <v>30,000,000</v>
+      <c r="I163">
+        <v>30000000</v>
       </c>
       <c r="J163" t="str">
         <v>차수민</v>
@@ -7008,7 +7008,7 @@
       <c r="H164" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I164" t="str">
+      <c r="I164">
         <v>0</v>
       </c>
     </row>
@@ -7037,8 +7037,8 @@
       <c r="H165" t="str">
         <v>일반용역</v>
       </c>
-      <c r="I165" t="str">
-        <v>150,000,000</v>
+      <c r="I165">
+        <v>150000000</v>
       </c>
       <c r="J165" t="str">
         <v>윤은희</v>

</xml_diff>